<commit_message>
Improvment of exel file
</commit_message>
<xml_diff>
--- a/src/test/test_data/SwagLabsData.xlsx
+++ b/src/test/test_data/SwagLabsData.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vazba_automatizacija_XIII_pom_Cucumber_EXCEL_SwagLabs\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D338EE56-8A3C-4AA6-84B2-D71DBA4B141E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575EA6E6-E83E-4390-89CD-0835EB2BCEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SwagLabs" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SwagLabs!$A$3:$G$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>tc_id</t>
   </si>
@@ -104,20 +107,35 @@
     <t>PRODUCTS</t>
   </si>
   <si>
-    <t xml:space="preserve">Epic sadface: Sorry, this user has been locked out.   </t>
-  </si>
-  <si>
     <t>Epic sadface: Username and password do not match any user in this service</t>
   </si>
   <si>
     <t>Epic sadface: Username is required</t>
+  </si>
+  <si>
+    <t>Epic sadface: Sorry, this user has been locked out.</t>
+  </si>
+  <si>
+    <t>testTypeLogout</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Test import data for "SwasLabs" project</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>logoutMessage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +159,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -151,18 +184,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -186,11 +219,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -201,7 +249,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -214,10 +262,142 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -226,21 +406,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -557,165 +763,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="69" customWidth="1"/>
+    <col min="1" max="1" width="10" style="21" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="15" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="16"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E10" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:G3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}"/>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>